<commit_message>
Rapor + Görev Mekanizması
</commit_message>
<xml_diff>
--- a/İHA Malzemeler.xlsx
+++ b/İHA Malzemeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\Desktop\IHA-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A5089C-5485-4598-9789-CC15DA336EF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74118692-68CA-428E-99E8-486B287B79C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Adet</t>
   </si>
@@ -76,9 +76,6 @@
     <t>HAKRC 40A x 4 2-5s Blheli-s Dshot600 Esc</t>
   </si>
   <si>
-    <t>Batarya 3S  2200 40C (+1 Tane Yedek)</t>
-  </si>
-  <si>
     <t>XBee Explorer USB</t>
   </si>
   <si>
@@ -152,13 +149,25 @@
   </si>
   <si>
     <t>1?</t>
+  </si>
+  <si>
+    <t>291,5 </t>
+  </si>
+  <si>
+    <t>708.28</t>
+  </si>
+  <si>
+    <t>Batarya 3S 4000 mAh 35C (+1 Tane Yedek)</t>
+  </si>
+  <si>
+    <t>Batarya 3S 2200 mAh 40C (+1 Tane Yedek)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +221,13 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -326,7 +342,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,6 +406,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -399,15 +421,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -424,6 +437,15 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -438,12 +460,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tablo1" displayName="Tablo1" ref="B1:E15" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B1:E15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tablo1" displayName="Tablo1" ref="B1:E16" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B1:E16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ürün Türkiye"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Toplam Fiyat(K.D.V. Dahil)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Toplam Ağırlık (gr)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Toplam Ağırlık (gr)" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Adet"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -451,10 +473,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tablo2" displayName="Tablo2" ref="A1:A12" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tablo2" displayName="Tablo2" ref="A1:A12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:A12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Alınma Durumu" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Alınma Durumu" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -723,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3">
         <v>628.02</v>
@@ -910,13 +932,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="10"/>
@@ -934,7 +956,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
         <v>443.75</v>
@@ -988,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="8">
         <v>576</v>
@@ -997,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="10"/>
@@ -1015,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11">
         <v>72.98</v>
@@ -1024,12 +1046,12 @@
         <v>12</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="11">
         <v>259.60000000000002</v>
@@ -1043,7 +1065,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="9">
         <v>576</v>
@@ -1070,6 +1092,20 @@
       <c r="E15" s="5">
         <f>SUBTOTAL(109,E2:E14)</f>
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="24">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1100,16 +1136,16 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -1217,10 +1253,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -1252,10 +1288,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -1287,10 +1323,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -1322,10 +1358,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -1357,10 +1393,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -1392,10 +1428,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -1427,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="18"/>
@@ -1462,10 +1498,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>

</xml_diff>